<commit_message>
made changes in scripts and added subscription model
</commit_message>
<xml_diff>
--- a/storage/durgesh/Graseed_grains.xlsx
+++ b/storage/durgesh/Graseed_grains.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,34 +495,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>7.85</v>
+        <v>42.72</v>
       </c>
       <c r="D2" t="n">
-        <v>3.15</v>
+        <v>17.14</v>
       </c>
       <c r="E2" t="n">
-        <v>1.35</v>
+        <v>7.32</v>
       </c>
       <c r="F2" t="n">
-        <v>0.21</v>
+        <v>1.16</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H2" t="n">
-        <v>0.03</v>
+        <v>0.14</v>
       </c>
       <c r="I2" t="n">
-        <v>15.39</v>
+        <v>83.70999999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>2.78</v>
+        <v>15.13</v>
       </c>
       <c r="K2" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="3">
@@ -533,31 +533,31 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>3.45</v>
+        <v>6.12</v>
       </c>
       <c r="D3" t="n">
-        <v>2.36</v>
+        <v>6.91</v>
       </c>
       <c r="E3" t="n">
-        <v>0.54</v>
+        <v>3.12</v>
       </c>
       <c r="F3" t="n">
-        <v>0.26</v>
+        <v>0.32</v>
       </c>
       <c r="G3" t="n">
         <v>0.01</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="I3" t="n">
-        <v>7.57</v>
+        <v>11</v>
       </c>
       <c r="J3" t="n">
-        <v>1.32</v>
+        <v>6.38</v>
       </c>
       <c r="K3" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="4">
@@ -568,31 +568,31 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>2.38</v>
+        <v>18.78</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>12.85</v>
       </c>
       <c r="E4" t="n">
-        <v>0.88</v>
+        <v>2.96</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1</v>
+        <v>1.4</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H4" t="n">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="I4" t="n">
-        <v>5.56</v>
+        <v>41.19</v>
       </c>
       <c r="J4" t="n">
-        <v>1.8</v>
+        <v>7.18</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5">
@@ -603,31 +603,31 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>4.74</v>
+        <v>12.97</v>
       </c>
       <c r="D5" t="n">
-        <v>3.71</v>
+        <v>10.89</v>
       </c>
       <c r="E5" t="n">
-        <v>0.78</v>
+        <v>4.78</v>
       </c>
       <c r="F5" t="n">
-        <v>0.28</v>
+        <v>0.53</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01</v>
+        <v>0.2</v>
       </c>
       <c r="I5" t="n">
-        <v>16.5</v>
+        <v>30.22</v>
       </c>
       <c r="J5" t="n">
-        <v>2.02</v>
+        <v>9.81</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="6">
@@ -638,31 +638,31 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>2.38</v>
+        <v>25.76</v>
       </c>
       <c r="D6" t="n">
-        <v>2.28</v>
+        <v>20.19</v>
       </c>
       <c r="E6" t="n">
-        <v>1.03</v>
+        <v>4.26</v>
       </c>
       <c r="F6" t="n">
-        <v>0.09</v>
+        <v>1.53</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H6" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="I6" t="n">
-        <v>5.53</v>
+        <v>89.76000000000001</v>
       </c>
       <c r="J6" t="n">
-        <v>2.11</v>
+        <v>10.96</v>
       </c>
       <c r="K6" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="7">
@@ -673,31 +673,31 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>5.51</v>
+        <v>12.93</v>
       </c>
       <c r="D7" t="n">
-        <v>4.39</v>
+        <v>12.41</v>
       </c>
       <c r="E7" t="n">
-        <v>1.81</v>
+        <v>5.6</v>
       </c>
       <c r="F7" t="n">
-        <v>0.27</v>
+        <v>0.5</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H7" t="n">
-        <v>0.01</v>
+        <v>0.23</v>
       </c>
       <c r="I7" t="n">
-        <v>28.2</v>
+        <v>30.05</v>
       </c>
       <c r="J7" t="n">
-        <v>3.74</v>
+        <v>11.46</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="8">
@@ -708,31 +708,31 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>9.94</v>
+        <v>5.32</v>
       </c>
       <c r="D8" t="n">
-        <v>6.41</v>
+        <v>5.89</v>
       </c>
       <c r="E8" t="n">
-        <v>2.33</v>
+        <v>2.67</v>
       </c>
       <c r="F8" t="n">
-        <v>0.34</v>
+        <v>0.27</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H8" t="n">
-        <v>0.01</v>
+        <v>0.31</v>
       </c>
       <c r="I8" t="n">
-        <v>37.78</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="J8" t="n">
-        <v>4.77</v>
+        <v>5.48</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="9">
@@ -740,31 +740,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>3.34</v>
+        <v>29.95</v>
       </c>
       <c r="D9" t="n">
-        <v>2.14</v>
+        <v>23.87</v>
       </c>
       <c r="E9" t="n">
-        <v>0.87</v>
+        <v>9.83</v>
       </c>
       <c r="F9" t="n">
-        <v>0.13</v>
+        <v>1.45</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H9" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="I9" t="n">
-        <v>6.94</v>
+        <v>153.36</v>
       </c>
       <c r="J9" t="n">
-        <v>1.81</v>
+        <v>20.33</v>
       </c>
       <c r="K9" t="n">
         <v>0.01</v>
@@ -778,31 +778,31 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>9.289999999999999</v>
+        <v>7.11</v>
       </c>
       <c r="D10" t="n">
-        <v>3.49</v>
+        <v>8.02</v>
       </c>
       <c r="E10" t="n">
-        <v>1.52</v>
+        <v>1.84</v>
       </c>
       <c r="F10" t="n">
-        <v>0.16</v>
+        <v>1.16</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="H10" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="I10" t="n">
-        <v>15.52</v>
+        <v>21.61</v>
       </c>
       <c r="J10" t="n">
-        <v>3.13</v>
+        <v>4.88</v>
       </c>
       <c r="K10" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="11">
@@ -810,34 +810,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>4.12</v>
+        <v>54.06</v>
       </c>
       <c r="D11" t="n">
-        <v>1.67</v>
+        <v>34.89</v>
       </c>
       <c r="E11" t="n">
-        <v>0.72</v>
+        <v>12.7</v>
       </c>
       <c r="F11" t="n">
-        <v>0.14</v>
+        <v>1.84</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H11" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I11" t="n">
-        <v>5.7</v>
+        <v>205.49</v>
       </c>
       <c r="J11" t="n">
-        <v>1.53</v>
+        <v>25.96</v>
       </c>
       <c r="K11" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="12">
@@ -848,31 +848,31 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>3.72</v>
+        <v>5.59</v>
       </c>
       <c r="D12" t="n">
-        <v>2.43</v>
+        <v>4.63</v>
       </c>
       <c r="E12" t="n">
-        <v>0.77</v>
+        <v>1.66</v>
       </c>
       <c r="F12" t="n">
-        <v>0.18</v>
+        <v>0.53</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="I12" t="n">
-        <v>9.550000000000001</v>
+        <v>9.81</v>
       </c>
       <c r="J12" t="n">
-        <v>1.75</v>
+        <v>3.84</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="13">
@@ -883,31 +883,31 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>2.24</v>
+        <v>7.88</v>
       </c>
       <c r="D13" t="n">
-        <v>2.05</v>
+        <v>6.34</v>
       </c>
       <c r="E13" t="n">
-        <v>0.52</v>
+        <v>1.67</v>
       </c>
       <c r="F13" t="n">
-        <v>0.19</v>
+        <v>0.72</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I13" t="n">
-        <v>6.03</v>
+        <v>14.33</v>
       </c>
       <c r="J13" t="n">
-        <v>1.19</v>
+        <v>4.15</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="14">
@@ -918,31 +918,31 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>5.6</v>
+        <v>18.15</v>
       </c>
       <c r="D14" t="n">
-        <v>3.4</v>
+        <v>11.65</v>
       </c>
       <c r="E14" t="n">
-        <v>1.46</v>
+        <v>4.75</v>
       </c>
       <c r="F14" t="n">
-        <v>0.13</v>
+        <v>0.68</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="I14" t="n">
-        <v>12.32</v>
+        <v>37.73</v>
       </c>
       <c r="J14" t="n">
-        <v>3</v>
+        <v>9.85</v>
       </c>
       <c r="K14" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="15">
@@ -950,34 +950,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>8.01</v>
+        <v>50.53</v>
       </c>
       <c r="D15" t="n">
-        <v>3.13</v>
+        <v>18.95</v>
       </c>
       <c r="E15" t="n">
-        <v>1.19</v>
+        <v>8.24</v>
       </c>
       <c r="F15" t="n">
-        <v>0.41</v>
+        <v>0.88</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="I15" t="n">
-        <v>23.82</v>
+        <v>84.41</v>
       </c>
       <c r="J15" t="n">
-        <v>2.67</v>
+        <v>17.02</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="16">
@@ -988,31 +988,31 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>2.92</v>
+        <v>22.41</v>
       </c>
       <c r="D16" t="n">
-        <v>0.95</v>
+        <v>9.1</v>
       </c>
       <c r="E16" t="n">
-        <v>0.3</v>
+        <v>3.94</v>
       </c>
       <c r="F16" t="n">
-        <v>0.19</v>
+        <v>0.78</v>
       </c>
       <c r="G16" t="n">
         <v>0.01</v>
       </c>
       <c r="H16" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="I16" t="n">
-        <v>3.81</v>
+        <v>30.98</v>
       </c>
       <c r="J16" t="n">
-        <v>0.83</v>
+        <v>8.31</v>
       </c>
       <c r="K16" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="17">
@@ -1023,31 +1023,31 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>2.62</v>
+        <v>20.21</v>
       </c>
       <c r="D17" t="n">
-        <v>1.18</v>
+        <v>13.22</v>
       </c>
       <c r="E17" t="n">
-        <v>0.45</v>
+        <v>4.18</v>
       </c>
       <c r="F17" t="n">
-        <v>0.15</v>
+        <v>0.98</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H17" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="I17" t="n">
-        <v>3.95</v>
+        <v>51.93</v>
       </c>
       <c r="J17" t="n">
-        <v>1.02</v>
+        <v>9.51</v>
       </c>
       <c r="K17" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="18">
@@ -1058,31 +1058,31 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>6.22</v>
       </c>
       <c r="D18" t="n">
-        <v>1.46</v>
+        <v>6.25</v>
       </c>
       <c r="E18" t="n">
-        <v>0.54</v>
+        <v>2.46</v>
       </c>
       <c r="F18" t="n">
-        <v>0.15</v>
+        <v>0.6</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H18" t="n">
-        <v>0.01</v>
+        <v>0.08</v>
       </c>
       <c r="I18" t="n">
-        <v>4.77</v>
+        <v>12.57</v>
       </c>
       <c r="J18" t="n">
-        <v>1.17</v>
+        <v>5.29</v>
       </c>
       <c r="K18" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="19">
@@ -1093,31 +1093,31 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>3.74</v>
+        <v>12.2</v>
       </c>
       <c r="D19" t="n">
-        <v>1.05</v>
+        <v>11.16</v>
       </c>
       <c r="E19" t="n">
-        <v>0.43</v>
+        <v>2.83</v>
       </c>
       <c r="F19" t="n">
-        <v>0.15</v>
+        <v>1.02</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H19" t="n">
         <v>0.02</v>
       </c>
       <c r="I19" t="n">
-        <v>4.14</v>
+        <v>32.81</v>
       </c>
       <c r="J19" t="n">
-        <v>0.99</v>
+        <v>6.45</v>
       </c>
       <c r="K19" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="20">
@@ -1125,34 +1125,34 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>1.88</v>
+        <v>30.45</v>
       </c>
       <c r="D20" t="n">
-        <v>0.76</v>
+        <v>18.52</v>
       </c>
       <c r="E20" t="n">
-        <v>0.31</v>
+        <v>7.92</v>
       </c>
       <c r="F20" t="n">
-        <v>0.11</v>
+        <v>0.73</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H20" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="I20" t="n">
-        <v>2.07</v>
+        <v>66.98999999999999</v>
       </c>
       <c r="J20" t="n">
-        <v>0.71</v>
+        <v>16.31</v>
       </c>
       <c r="K20" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="21">
@@ -1163,31 +1163,31 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>5.4</v>
+        <v>8.68</v>
       </c>
       <c r="D21" t="n">
-        <v>1.73</v>
+        <v>7.93</v>
       </c>
       <c r="E21" t="n">
-        <v>0.57</v>
+        <v>3.45</v>
       </c>
       <c r="F21" t="n">
-        <v>0.22</v>
+        <v>0.47</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H21" t="n">
         <v>0.02</v>
       </c>
       <c r="I21" t="n">
-        <v>7.13</v>
+        <v>17.85</v>
       </c>
       <c r="J21" t="n">
-        <v>1.3</v>
+        <v>7.17</v>
       </c>
       <c r="K21" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="22">
@@ -1195,34 +1195,34 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>2.05</v>
+        <v>43.55</v>
       </c>
       <c r="D22" t="n">
-        <v>1.34</v>
+        <v>17.03</v>
       </c>
       <c r="E22" t="n">
-        <v>0.57</v>
+        <v>6.48</v>
       </c>
       <c r="F22" t="n">
-        <v>0.12</v>
+        <v>2.22</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="I22" t="n">
-        <v>3.7</v>
+        <v>129.55</v>
       </c>
       <c r="J22" t="n">
-        <v>1.21</v>
+        <v>14.53</v>
       </c>
       <c r="K22" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="23">
@@ -1233,31 +1233,31 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>2.81</v>
+        <v>15.86</v>
       </c>
       <c r="D23" t="n">
-        <v>1.37</v>
+        <v>5.18</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5600000000000001</v>
+        <v>1.61</v>
       </c>
       <c r="F23" t="n">
-        <v>0.16</v>
+        <v>1.01</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="H23" t="n">
-        <v>0.02</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I23" t="n">
-        <v>4.88</v>
+        <v>20.74</v>
       </c>
       <c r="J23" t="n">
-        <v>1.25</v>
+        <v>4.51</v>
       </c>
       <c r="K23" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="24">
@@ -1268,31 +1268,31 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>2.98</v>
+        <v>14.23</v>
       </c>
       <c r="D24" t="n">
-        <v>0.99</v>
+        <v>6.44</v>
       </c>
       <c r="E24" t="n">
-        <v>0.4</v>
+        <v>2.46</v>
       </c>
       <c r="F24" t="n">
-        <v>0.14</v>
+        <v>0.8</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H24" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I24" t="n">
-        <v>3.46</v>
+        <v>21.48</v>
       </c>
       <c r="J24" t="n">
-        <v>0.95</v>
+        <v>5.54</v>
       </c>
       <c r="K24" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="25">
@@ -1303,31 +1303,31 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>2.21</v>
+        <v>16.32</v>
       </c>
       <c r="D25" t="n">
-        <v>1.27</v>
+        <v>7.96</v>
       </c>
       <c r="E25" t="n">
-        <v>0.44</v>
+        <v>2.96</v>
       </c>
       <c r="F25" t="n">
-        <v>0.17</v>
+        <v>0.83</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="I25" t="n">
-        <v>3.95</v>
+        <v>25.93</v>
       </c>
       <c r="J25" t="n">
-        <v>1.03</v>
+        <v>6.37</v>
       </c>
       <c r="K25" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="26">
@@ -1338,31 +1338,31 @@
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>6.31</v>
+        <v>7.48</v>
       </c>
       <c r="D26" t="n">
-        <v>2.48</v>
+        <v>6.84</v>
       </c>
       <c r="E26" t="n">
-        <v>0.72</v>
+        <v>3.13</v>
       </c>
       <c r="F26" t="n">
-        <v>0.23</v>
+        <v>0.39</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H26" t="n">
-        <v>0.02</v>
+        <v>0.22</v>
       </c>
       <c r="I26" t="n">
-        <v>10</v>
+        <v>13.43</v>
       </c>
       <c r="J26" t="n">
-        <v>1.62</v>
+        <v>6.47</v>
       </c>
       <c r="K26" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="27">
@@ -1373,31 +1373,31 @@
         <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>2.7</v>
+        <v>20.35</v>
       </c>
       <c r="D27" t="n">
-        <v>1.93</v>
+        <v>5.71</v>
       </c>
       <c r="E27" t="n">
-        <v>0.31</v>
+        <v>2.36</v>
       </c>
       <c r="F27" t="n">
-        <v>0.26</v>
+        <v>0.84</v>
       </c>
       <c r="G27" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H27" t="n">
-        <v>0.01</v>
+        <v>0.13</v>
       </c>
       <c r="I27" t="n">
-        <v>5.49</v>
+        <v>22.51</v>
       </c>
       <c r="J27" t="n">
-        <v>0.97</v>
+        <v>5.37</v>
       </c>
       <c r="K27" t="n">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="28">
@@ -1408,31 +1408,31 @@
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>3.02</v>
+        <v>10.24</v>
       </c>
       <c r="D28" t="n">
-        <v>1.79</v>
+        <v>4.14</v>
       </c>
       <c r="E28" t="n">
-        <v>0.74</v>
+        <v>1.66</v>
       </c>
       <c r="F28" t="n">
-        <v>0.15</v>
+        <v>0.6</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H28" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="I28" t="n">
-        <v>5.49</v>
+        <v>11.24</v>
       </c>
       <c r="J28" t="n">
-        <v>1.56</v>
+        <v>3.87</v>
       </c>
       <c r="K28" t="n">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="29">
@@ -1440,34 +1440,34 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>5.2</v>
+        <v>29.36</v>
       </c>
       <c r="D29" t="n">
-        <v>1.06</v>
+        <v>9.390000000000001</v>
       </c>
       <c r="E29" t="n">
-        <v>0.32</v>
+        <v>3.09</v>
       </c>
       <c r="F29" t="n">
-        <v>0.29</v>
+        <v>1.18</v>
       </c>
       <c r="G29" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01</v>
+        <v>0.09</v>
       </c>
       <c r="I29" t="n">
-        <v>5.46</v>
+        <v>38.76</v>
       </c>
       <c r="J29" t="n">
-        <v>1.02</v>
+        <v>7.06</v>
       </c>
       <c r="K29" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="30">
@@ -1478,31 +1478,31 @@
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>4.39</v>
+        <v>11.17</v>
       </c>
       <c r="D30" t="n">
-        <v>1.46</v>
+        <v>7.31</v>
       </c>
       <c r="E30" t="n">
-        <v>0.58</v>
+        <v>3.08</v>
       </c>
       <c r="F30" t="n">
-        <v>0.16</v>
+        <v>0.63</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H30" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="I30" t="n">
-        <v>5.45</v>
+        <v>20.11</v>
       </c>
       <c r="J30" t="n">
-        <v>1.26</v>
+        <v>6.57</v>
       </c>
       <c r="K30" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="31">
@@ -1513,31 +1513,31 @@
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>1.96</v>
+        <v>8.58</v>
       </c>
       <c r="D31" t="n">
-        <v>1.17</v>
+        <v>4.1</v>
       </c>
       <c r="E31" t="n">
-        <v>0.33</v>
+        <v>1.66</v>
       </c>
       <c r="F31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H31" t="n">
         <v>0.15</v>
       </c>
-      <c r="G31" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0.01</v>
-      </c>
       <c r="I31" t="n">
-        <v>3.36</v>
+        <v>10.11</v>
       </c>
       <c r="J31" t="n">
-        <v>0.86</v>
+        <v>3.86</v>
       </c>
       <c r="K31" t="n">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="32">
@@ -1548,31 +1548,31 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>4.63</v>
+        <v>15.26</v>
       </c>
       <c r="D32" t="n">
-        <v>2.2</v>
+        <v>7.44</v>
       </c>
       <c r="E32" t="n">
-        <v>0.75</v>
+        <v>3.06</v>
       </c>
       <c r="F32" t="n">
-        <v>0.27</v>
+        <v>0.87</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H32" t="n">
-        <v>0.01</v>
+        <v>0.09</v>
       </c>
       <c r="I32" t="n">
-        <v>10.06</v>
+        <v>26.53</v>
       </c>
       <c r="J32" t="n">
-        <v>1.69</v>
+        <v>6.8</v>
       </c>
       <c r="K32" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="33">
@@ -1583,31 +1583,31 @@
         <v>0</v>
       </c>
       <c r="C33" t="n">
+        <v>16.19</v>
+      </c>
+      <c r="D33" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="E33" t="n">
         <v>2.16</v>
       </c>
-      <c r="D33" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0.47</v>
-      </c>
       <c r="F33" t="n">
-        <v>0.11</v>
+        <v>0.74</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H33" t="n">
-        <v>0.02</v>
+        <v>0.13</v>
       </c>
       <c r="I33" t="n">
-        <v>3.07</v>
+        <v>18.82</v>
       </c>
       <c r="J33" t="n">
-        <v>1.03</v>
+        <v>5.17</v>
       </c>
       <c r="K33" t="n">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="34">
@@ -1618,31 +1618,31 @@
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>1.96</v>
+        <v>12.03</v>
       </c>
       <c r="D34" t="n">
-        <v>1.67</v>
+        <v>6.9</v>
       </c>
       <c r="E34" t="n">
-        <v>0.49</v>
+        <v>2.37</v>
       </c>
       <c r="F34" t="n">
-        <v>0.13</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H34" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="I34" t="n">
-        <v>3.88</v>
+        <v>21.48</v>
       </c>
       <c r="J34" t="n">
-        <v>1.07</v>
+        <v>5.58</v>
       </c>
       <c r="K34" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="35">
@@ -1653,31 +1653,31 @@
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>3.25</v>
+        <v>7.41</v>
       </c>
       <c r="D35" t="n">
-        <v>2.27</v>
+        <v>4.74</v>
       </c>
       <c r="E35" t="n">
-        <v>0.43</v>
+        <v>1.52</v>
       </c>
       <c r="F35" t="n">
-        <v>0.31</v>
+        <v>0.88</v>
       </c>
       <c r="G35" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="I35" t="n">
-        <v>6.94</v>
+        <v>13.46</v>
       </c>
       <c r="J35" t="n">
-        <v>1.22</v>
+        <v>3.86</v>
       </c>
       <c r="K35" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="36">
@@ -1688,31 +1688,31 @@
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>4.83</v>
+        <v>9.01</v>
       </c>
       <c r="D36" t="n">
-        <v>2.97</v>
+        <v>7.01</v>
       </c>
       <c r="E36" t="n">
-        <v>1.01</v>
+        <v>2.36</v>
       </c>
       <c r="F36" t="n">
-        <v>0.17</v>
+        <v>0.65</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H36" t="n">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="I36" t="n">
-        <v>9.93</v>
+        <v>15.06</v>
       </c>
       <c r="J36" t="n">
-        <v>2.09</v>
+        <v>5.19</v>
       </c>
       <c r="K36" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="37">
@@ -1723,31 +1723,31 @@
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>3.7</v>
+        <v>9.08</v>
       </c>
       <c r="D37" t="n">
-        <v>2.28</v>
+        <v>4.96</v>
       </c>
       <c r="E37" t="n">
-        <v>0.93</v>
+        <v>1.71</v>
       </c>
       <c r="F37" t="n">
-        <v>0.14</v>
+        <v>0.74</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H37" t="n">
-        <v>0.03</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I37" t="n">
-        <v>6.63</v>
+        <v>12.13</v>
       </c>
       <c r="J37" t="n">
-        <v>1.93</v>
+        <v>4</v>
       </c>
       <c r="K37" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="38">
@@ -1755,34 +1755,34 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>8</v>
+        <v>34.34</v>
       </c>
       <c r="D38" t="n">
-        <v>3.81</v>
+        <v>13.49</v>
       </c>
       <c r="E38" t="n">
-        <v>1.1</v>
+        <v>3.93</v>
       </c>
       <c r="F38" t="n">
-        <v>0.33</v>
+        <v>1.25</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H38" t="n">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="I38" t="n">
-        <v>17.18</v>
+        <v>54.39</v>
       </c>
       <c r="J38" t="n">
-        <v>2.4</v>
+        <v>8.789999999999999</v>
       </c>
       <c r="K38" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="39">
@@ -1793,31 +1793,31 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>1.82</v>
+        <v>14.69</v>
       </c>
       <c r="D39" t="n">
-        <v>1.35</v>
+        <v>10.47</v>
       </c>
       <c r="E39" t="n">
-        <v>0.34</v>
+        <v>1.69</v>
       </c>
       <c r="F39" t="n">
-        <v>0.18</v>
+        <v>1.42</v>
       </c>
       <c r="G39" t="n">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="H39" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="I39" t="n">
-        <v>3.27</v>
+        <v>29.85</v>
       </c>
       <c r="J39" t="n">
-        <v>0.86</v>
+        <v>5.26</v>
       </c>
       <c r="K39" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="40">
@@ -1828,31 +1828,31 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>11.23</v>
+        <v>6.45</v>
       </c>
       <c r="D40" t="n">
-        <v>6.02</v>
+        <v>3.05</v>
       </c>
       <c r="E40" t="n">
-        <v>1.23</v>
+        <v>1.19</v>
       </c>
       <c r="F40" t="n">
-        <v>0.47</v>
+        <v>0.59</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H40" t="n">
-        <v>0.01</v>
+        <v>0.08</v>
       </c>
       <c r="I40" t="n">
-        <v>29.12</v>
+        <v>7.61</v>
       </c>
       <c r="J40" t="n">
-        <v>2.83</v>
+        <v>2.85</v>
       </c>
       <c r="K40" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="41">
@@ -1863,31 +1863,31 @@
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>3.09</v>
+        <v>7.78</v>
       </c>
       <c r="D41" t="n">
-        <v>2.42</v>
+        <v>3.1</v>
       </c>
       <c r="E41" t="n">
-        <v>0.62</v>
+        <v>1.2</v>
       </c>
       <c r="F41" t="n">
-        <v>0.29</v>
+        <v>0.64</v>
       </c>
       <c r="G41" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="I41" t="n">
-        <v>8.69</v>
+        <v>8.44</v>
       </c>
       <c r="J41" t="n">
-        <v>1.44</v>
+        <v>2.96</v>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="42">
@@ -1898,31 +1898,31 @@
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>7.7</v>
+        <v>16.42</v>
       </c>
       <c r="D42" t="n">
-        <v>2.82</v>
+        <v>9.720000000000001</v>
       </c>
       <c r="E42" t="n">
-        <v>0.72</v>
+        <v>4.01</v>
       </c>
       <c r="F42" t="n">
-        <v>0.46</v>
+        <v>0.8</v>
       </c>
       <c r="G42" t="n">
         <v>0.01</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="I42" t="n">
-        <v>22.21</v>
+        <v>29.85</v>
       </c>
       <c r="J42" t="n">
-        <v>2.12</v>
+        <v>8.470000000000001</v>
       </c>
       <c r="K42" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="43">
@@ -1930,34 +1930,34 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>7.74</v>
+        <v>28.29</v>
       </c>
       <c r="D43" t="n">
-        <v>4.6</v>
+        <v>5.74</v>
       </c>
       <c r="E43" t="n">
-        <v>1.42</v>
+        <v>1.74</v>
       </c>
       <c r="F43" t="n">
-        <v>0.26</v>
+        <v>1.6</v>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="H43" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="I43" t="n">
-        <v>21.78</v>
+        <v>29.72</v>
       </c>
       <c r="J43" t="n">
-        <v>2.99</v>
+        <v>5.54</v>
       </c>
       <c r="K43" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="44">
@@ -1968,31 +1968,31 @@
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>9.789999999999999</v>
+        <v>5.92</v>
       </c>
       <c r="D44" t="n">
-        <v>4.54</v>
+        <v>4.33</v>
       </c>
       <c r="E44" t="n">
-        <v>1.42</v>
+        <v>1.05</v>
       </c>
       <c r="F44" t="n">
-        <v>0.24</v>
+        <v>0.88</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="H44" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I44" t="n">
-        <v>20.68</v>
+        <v>9.74</v>
       </c>
       <c r="J44" t="n">
-        <v>2.98</v>
+        <v>3.22</v>
       </c>
       <c r="K44" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="45">
@@ -2003,31 +2003,31 @@
         <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>3.11</v>
+        <v>8.84</v>
       </c>
       <c r="D45" t="n">
-        <v>2.07</v>
+        <v>6.11</v>
       </c>
       <c r="E45" t="n">
-        <v>0.71</v>
+        <v>2.64</v>
       </c>
       <c r="F45" t="n">
-        <v>0.18</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H45" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="I45" t="n">
-        <v>7.02</v>
+        <v>15.46</v>
       </c>
       <c r="J45" t="n">
-        <v>1.53</v>
+        <v>5.69</v>
       </c>
       <c r="K45" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="46">
@@ -2038,31 +2038,31 @@
         <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>13.55</v>
+        <v>23.9</v>
       </c>
       <c r="D46" t="n">
-        <v>7.36</v>
+        <v>7.96</v>
       </c>
       <c r="E46" t="n">
-        <v>1.06</v>
+        <v>3.15</v>
       </c>
       <c r="F46" t="n">
-        <v>0.72</v>
+        <v>0.86</v>
       </c>
       <c r="G46" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="I46" t="n">
-        <v>41.25</v>
+        <v>29.62</v>
       </c>
       <c r="J46" t="n">
-        <v>2.88</v>
+        <v>6.87</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="47">
@@ -2073,31 +2073,31 @@
         <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>7.84</v>
+        <v>10.67</v>
       </c>
       <c r="D47" t="n">
-        <v>3.14</v>
+        <v>6.37</v>
       </c>
       <c r="E47" t="n">
-        <v>0.84</v>
+        <v>1.8</v>
       </c>
       <c r="F47" t="n">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H47" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I47" t="n">
-        <v>12</v>
+        <v>18.25</v>
       </c>
       <c r="J47" t="n">
-        <v>1.9</v>
+        <v>4.69</v>
       </c>
       <c r="K47" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="48">
@@ -2108,31 +2108,31 @@
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>3.62</v>
+        <v>25.17</v>
       </c>
       <c r="D48" t="n">
-        <v>1.65</v>
+        <v>11.95</v>
       </c>
       <c r="E48" t="n">
-        <v>0.51</v>
+        <v>4.06</v>
       </c>
       <c r="F48" t="n">
-        <v>0.18</v>
+        <v>1.47</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H48" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="I48" t="n">
-        <v>5.9</v>
+        <v>54.69</v>
       </c>
       <c r="J48" t="n">
-        <v>1.16</v>
+        <v>9.17</v>
       </c>
       <c r="K48" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="49">
@@ -2143,31 +2143,31 @@
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>4.6</v>
+        <v>11.74</v>
       </c>
       <c r="D49" t="n">
-        <v>1.5</v>
+        <v>6.18</v>
       </c>
       <c r="E49" t="n">
-        <v>0.64</v>
+        <v>2.53</v>
       </c>
       <c r="F49" t="n">
-        <v>0.15</v>
+        <v>0.62</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H49" t="n">
-        <v>0.03</v>
+        <v>0.13</v>
       </c>
       <c r="I49" t="n">
-        <v>5.46</v>
+        <v>16.72</v>
       </c>
       <c r="J49" t="n">
-        <v>1.39</v>
+        <v>5.58</v>
       </c>
       <c r="K49" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="50">
@@ -2178,31 +2178,31 @@
         <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>2.93</v>
+        <v>10.67</v>
       </c>
       <c r="D50" t="n">
-        <v>1.05</v>
+        <v>9.1</v>
       </c>
       <c r="E50" t="n">
-        <v>0.34</v>
+        <v>2.67</v>
       </c>
       <c r="F50" t="n">
-        <v>0.21</v>
+        <v>0.72</v>
       </c>
       <c r="G50" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H50" t="n">
-        <v>0.01</v>
+        <v>0.09</v>
       </c>
       <c r="I50" t="n">
-        <v>4.36</v>
+        <v>21.08</v>
       </c>
       <c r="J50" t="n">
-        <v>0.9</v>
+        <v>5.81</v>
       </c>
       <c r="K50" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="51">
@@ -2213,31 +2213,31 @@
         <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>10.02</v>
+        <v>17.69</v>
       </c>
       <c r="D51" t="n">
-        <v>6.51</v>
+        <v>12.37</v>
       </c>
       <c r="E51" t="n">
-        <v>0.98</v>
+        <v>2.33</v>
       </c>
       <c r="F51" t="n">
-        <v>0.5600000000000001</v>
+        <v>1.66</v>
       </c>
       <c r="G51" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="H51" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="I51" t="n">
-        <v>33.84</v>
+        <v>37.77</v>
       </c>
       <c r="J51" t="n">
-        <v>2.5</v>
+        <v>6.62</v>
       </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="52">
@@ -2248,31 +2248,31 @@
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>2.62</v>
+        <v>26.26</v>
       </c>
       <c r="D52" t="n">
-        <v>1.76</v>
+        <v>16.14</v>
       </c>
       <c r="E52" t="n">
-        <v>0.5</v>
+        <v>5.48</v>
       </c>
       <c r="F52" t="n">
-        <v>0.17</v>
+        <v>0.92</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H52" t="n">
-        <v>0.01</v>
+        <v>0.14</v>
       </c>
       <c r="I52" t="n">
-        <v>4.94</v>
+        <v>54.02</v>
       </c>
       <c r="J52" t="n">
-        <v>1.14</v>
+        <v>11.38</v>
       </c>
       <c r="K52" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="53">
@@ -2283,31 +2283,31 @@
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>7.92</v>
+        <v>20.11</v>
       </c>
       <c r="D53" t="n">
-        <v>2.86</v>
+        <v>12.39</v>
       </c>
       <c r="E53" t="n">
-        <v>0.6899999999999999</v>
+        <v>5.05</v>
       </c>
       <c r="F53" t="n">
-        <v>0.35</v>
+        <v>0.75</v>
       </c>
       <c r="G53" t="n">
         <v>0.01</v>
       </c>
       <c r="H53" t="n">
-        <v>0.01</v>
+        <v>0.16</v>
       </c>
       <c r="I53" t="n">
-        <v>13.38</v>
+        <v>36.04</v>
       </c>
       <c r="J53" t="n">
-        <v>1.72</v>
+        <v>10.48</v>
       </c>
       <c r="K53" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="54">
@@ -2315,34 +2315,34 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" t="n">
-        <v>5.4</v>
+        <v>43.48</v>
       </c>
       <c r="D54" t="n">
-        <v>2.52</v>
+        <v>20.73</v>
       </c>
       <c r="E54" t="n">
-        <v>0.89</v>
+        <v>5.99</v>
       </c>
       <c r="F54" t="n">
-        <v>0.25</v>
+        <v>1.8</v>
       </c>
       <c r="G54" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H54" t="n">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="I54" t="n">
-        <v>10.84</v>
+        <v>93.42</v>
       </c>
       <c r="J54" t="n">
-        <v>1.94</v>
+        <v>13.03</v>
       </c>
       <c r="K54" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="55">
@@ -2353,31 +2353,31 @@
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>5.06</v>
+        <v>6.28</v>
       </c>
       <c r="D55" t="n">
-        <v>3.32</v>
+        <v>2.98</v>
       </c>
       <c r="E55" t="n">
-        <v>0.8100000000000001</v>
+        <v>1.22</v>
       </c>
       <c r="F55" t="n">
-        <v>0.31</v>
+        <v>0.47</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H55" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="I55" t="n">
-        <v>14.24</v>
+        <v>6.75</v>
       </c>
       <c r="J55" t="n">
-        <v>1.83</v>
+        <v>2.89</v>
       </c>
       <c r="K55" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="56">
@@ -2388,31 +2388,31 @@
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>1.98</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="D56" t="n">
-        <v>1.23</v>
+        <v>7.34</v>
       </c>
       <c r="E56" t="n">
-        <v>0.55</v>
+        <v>1.83</v>
       </c>
       <c r="F56" t="n">
-        <v>0.09</v>
+        <v>0.99</v>
       </c>
       <c r="G56" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="H56" t="n">
         <v>0.04</v>
       </c>
       <c r="I56" t="n">
-        <v>2.52</v>
+        <v>17.79</v>
       </c>
       <c r="J56" t="n">
-        <v>1.16</v>
+        <v>4.67</v>
       </c>
       <c r="K56" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="57">
@@ -2420,34 +2420,34 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57" t="n">
-        <v>4.21</v>
+        <v>61.07</v>
       </c>
       <c r="D57" t="n">
-        <v>3.02</v>
+        <v>32.76</v>
       </c>
       <c r="E57" t="n">
-        <v>0.52</v>
+        <v>6.71</v>
       </c>
       <c r="F57" t="n">
-        <v>0.32</v>
+        <v>2.56</v>
       </c>
       <c r="G57" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="H57" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="I57" t="n">
-        <v>10.21</v>
+        <v>158.38</v>
       </c>
       <c r="J57" t="n">
-        <v>1.37</v>
+        <v>15.38</v>
       </c>
       <c r="K57" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="58">
@@ -2458,31 +2458,31 @@
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>14.4</v>
+        <v>5.59</v>
       </c>
       <c r="D58" t="n">
-        <v>4.09</v>
+        <v>4.14</v>
       </c>
       <c r="E58" t="n">
-        <v>1.2</v>
+        <v>0.93</v>
       </c>
       <c r="F58" t="n">
-        <v>0.28</v>
+        <v>0.86</v>
       </c>
       <c r="G58" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="H58" t="n">
         <v>0.03</v>
       </c>
       <c r="I58" t="n">
-        <v>22.04</v>
+        <v>8.91</v>
       </c>
       <c r="J58" t="n">
-        <v>2.64</v>
+        <v>2.94</v>
       </c>
       <c r="K58" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="59">
@@ -2493,31 +2493,31 @@
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>3.5</v>
+        <v>16.79</v>
       </c>
       <c r="D59" t="n">
-        <v>1.91</v>
+        <v>13.18</v>
       </c>
       <c r="E59" t="n">
-        <v>0.62</v>
+        <v>3.39</v>
       </c>
       <c r="F59" t="n">
-        <v>0.15</v>
+        <v>1.6</v>
       </c>
       <c r="G59" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H59" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="I59" t="n">
-        <v>5.93</v>
+        <v>47.24</v>
       </c>
       <c r="J59" t="n">
-        <v>1.36</v>
+        <v>7.84</v>
       </c>
       <c r="K59" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="60">
@@ -2525,34 +2525,34 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60" t="n">
-        <v>20.67</v>
+        <v>41.86</v>
       </c>
       <c r="D60" t="n">
-        <v>7.22</v>
+        <v>15.32</v>
       </c>
       <c r="E60" t="n">
-        <v>2.08</v>
+        <v>3.93</v>
       </c>
       <c r="F60" t="n">
-        <v>0.35</v>
+        <v>2.5</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="I60" t="n">
-        <v>40.23</v>
+        <v>120.81</v>
       </c>
       <c r="J60" t="n">
-        <v>4.35</v>
+        <v>11.5</v>
       </c>
       <c r="K60" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="61">
@@ -2560,34 +2560,34 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C61" t="n">
-        <v>8</v>
+        <v>42.09</v>
       </c>
       <c r="D61" t="n">
-        <v>3.4</v>
+        <v>25.03</v>
       </c>
       <c r="E61" t="n">
-        <v>1.17</v>
+        <v>7.73</v>
       </c>
       <c r="F61" t="n">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="G61" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H61" t="n">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="I61" t="n">
-        <v>12.3</v>
+        <v>118.48</v>
       </c>
       <c r="J61" t="n">
-        <v>2.47</v>
+        <v>16.24</v>
       </c>
       <c r="K61" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="62">
@@ -2595,34 +2595,34 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>3.33</v>
+        <v>53.22</v>
       </c>
       <c r="D62" t="n">
-        <v>1.93</v>
+        <v>24.67</v>
       </c>
       <c r="E62" t="n">
-        <v>0.37</v>
+        <v>7.73</v>
       </c>
       <c r="F62" t="n">
-        <v>0.35</v>
+        <v>1.32</v>
       </c>
       <c r="G62" t="n">
         <v>0.01</v>
       </c>
       <c r="H62" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="I62" t="n">
-        <v>7.87</v>
+        <v>112.47</v>
       </c>
       <c r="J62" t="n">
-        <v>1.17</v>
+        <v>16.19</v>
       </c>
       <c r="K62" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="63">
@@ -2633,31 +2633,31 @@
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>4.69</v>
+        <v>16.92</v>
       </c>
       <c r="D63" t="n">
-        <v>2.22</v>
+        <v>11.23</v>
       </c>
       <c r="E63" t="n">
-        <v>0.39</v>
+        <v>3.85</v>
       </c>
       <c r="F63" t="n">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="G63" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H63" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I63" t="n">
-        <v>8.74</v>
+        <v>38.16</v>
       </c>
       <c r="J63" t="n">
-        <v>1.21</v>
+        <v>8.32</v>
       </c>
       <c r="K63" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="64">
@@ -2665,34 +2665,34 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>9.720000000000001</v>
+        <v>73.7</v>
       </c>
       <c r="D64" t="n">
-        <v>5.12</v>
+        <v>40.04</v>
       </c>
       <c r="E64" t="n">
-        <v>0.83</v>
+        <v>5.79</v>
       </c>
       <c r="F64" t="n">
-        <v>0.5</v>
+        <v>3.91</v>
       </c>
       <c r="G64" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H64" t="n">
         <v>0.01</v>
       </c>
       <c r="I64" t="n">
-        <v>24.75</v>
+        <v>224.37</v>
       </c>
       <c r="J64" t="n">
-        <v>2.25</v>
+        <v>15.67</v>
       </c>
       <c r="K64" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="65">
@@ -2703,31 +2703,31 @@
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>8.58</v>
+        <v>9.08</v>
       </c>
       <c r="D65" t="n">
-        <v>2.82</v>
+        <v>7.23</v>
       </c>
       <c r="E65" t="n">
-        <v>0.77</v>
+        <v>2.1</v>
       </c>
       <c r="F65" t="n">
-        <v>0.38</v>
+        <v>1.34</v>
       </c>
       <c r="G65" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H65" t="n">
         <v>0.01</v>
       </c>
-      <c r="H65" t="n">
-        <v>0</v>
-      </c>
       <c r="I65" t="n">
-        <v>15.8</v>
+        <v>27.63</v>
       </c>
       <c r="J65" t="n">
-        <v>1.83</v>
+        <v>5.61</v>
       </c>
       <c r="K65" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="66">
@@ -2735,34 +2735,34 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66" t="n">
-        <v>4.45</v>
+        <v>42.65</v>
       </c>
       <c r="D66" t="n">
-        <v>1.12</v>
+        <v>17.09</v>
       </c>
       <c r="E66" t="n">
-        <v>0.4</v>
+        <v>4.59</v>
       </c>
       <c r="F66" t="n">
-        <v>0.18</v>
+        <v>1.61</v>
       </c>
       <c r="G66" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H66" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I66" t="n">
-        <v>4.93</v>
+        <v>65.26000000000001</v>
       </c>
       <c r="J66" t="n">
-        <v>1.01</v>
+        <v>10.35</v>
       </c>
       <c r="K66" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="67">
@@ -2773,31 +2773,31 @@
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>13.39</v>
+        <v>19.68</v>
       </c>
       <c r="D67" t="n">
-        <v>6.68</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="E67" t="n">
-        <v>1.82</v>
+        <v>2.75</v>
       </c>
       <c r="F67" t="n">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="G67" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H67" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="I67" t="n">
-        <v>36.89</v>
+        <v>32.11</v>
       </c>
       <c r="J67" t="n">
-        <v>3.84</v>
+        <v>6.3</v>
       </c>
       <c r="K67" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="68">
@@ -2808,31 +2808,31 @@
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>4.3</v>
+        <v>5.45</v>
       </c>
       <c r="D68" t="n">
-        <v>1.17</v>
+        <v>4.37</v>
       </c>
       <c r="E68" t="n">
-        <v>0.43</v>
+        <v>1.93</v>
       </c>
       <c r="F68" t="n">
-        <v>0.17</v>
+        <v>0.4</v>
       </c>
       <c r="G68" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H68" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="I68" t="n">
-        <v>4.81</v>
+        <v>7.68</v>
       </c>
       <c r="J68" t="n">
-        <v>1.09</v>
+        <v>4.06</v>
       </c>
       <c r="K68" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="69">
@@ -2843,31 +2843,31 @@
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>13.6</v>
+        <v>25.03</v>
       </c>
       <c r="D69" t="n">
-        <v>5.71</v>
+        <v>8.17</v>
       </c>
       <c r="E69" t="n">
-        <v>1.95</v>
+        <v>3.51</v>
       </c>
       <c r="F69" t="n">
-        <v>0.21</v>
+        <v>0.83</v>
       </c>
       <c r="G69" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H69" t="n">
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
       <c r="I69" t="n">
-        <v>25.14</v>
+        <v>29.69</v>
       </c>
       <c r="J69" t="n">
-        <v>4.03</v>
+        <v>7.58</v>
       </c>
       <c r="K69" t="n">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="70">
@@ -2878,31 +2878,1046 @@
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>2.15</v>
+        <v>15.92</v>
       </c>
       <c r="D70" t="n">
+        <v>5.73</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="F70" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="I70" t="n">
+        <v>23.7</v>
+      </c>
+      <c r="J70" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0</v>
+      </c>
+      <c r="C71" t="n">
+        <v>8.31</v>
+      </c>
+      <c r="D71" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="E71" t="n">
         <v>1.33</v>
       </c>
-      <c r="E70" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="F70" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="G70" t="n">
-        <v>0</v>
-      </c>
-      <c r="H70" t="n">
-        <v>0</v>
-      </c>
-      <c r="I70" t="n">
-        <v>3.37</v>
-      </c>
-      <c r="J70" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="K70" t="n">
+      <c r="F71" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I71" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="J71" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0</v>
+      </c>
+      <c r="C72" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="D72" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="I72" t="n">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="J72" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" t="n">
+        <v>54.49</v>
+      </c>
+      <c r="D73" t="n">
+        <v>35.43</v>
+      </c>
+      <c r="E73" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="F73" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I73" t="n">
+        <v>184.04</v>
+      </c>
+      <c r="J73" t="n">
+        <v>13.59</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0</v>
+      </c>
+      <c r="C74" t="n">
+        <v>7.18</v>
+      </c>
+      <c r="D74" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="I74" t="n">
+        <v>8.380000000000001</v>
+      </c>
+      <c r="J74" t="n">
+        <v>3.91</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0</v>
+      </c>
+      <c r="C75" t="n">
+        <v>14.23</v>
+      </c>
+      <c r="D75" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="E75" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="I75" t="n">
+        <v>26.89</v>
+      </c>
+      <c r="J75" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0</v>
+      </c>
+      <c r="C76" t="n">
+        <v>7.65</v>
+      </c>
+      <c r="D76" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="E76" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I76" t="n">
+        <v>17.49</v>
+      </c>
+      <c r="J76" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" t="n">
+        <v>43.09</v>
+      </c>
+      <c r="D77" t="n">
+        <v>15.57</v>
+      </c>
+      <c r="E77" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="F77" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="I77" t="n">
+        <v>72.77</v>
+      </c>
+      <c r="J77" t="n">
+        <v>9.380000000000001</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C78" t="n">
+        <v>29.39</v>
+      </c>
+      <c r="D78" t="n">
+        <v>13.7</v>
+      </c>
+      <c r="E78" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="F78" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="I78" t="n">
+        <v>58.94</v>
+      </c>
+      <c r="J78" t="n">
+        <v>10.57</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C79" t="n">
+        <v>27.49</v>
+      </c>
+      <c r="D79" t="n">
+        <v>18.08</v>
+      </c>
+      <c r="E79" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="F79" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="I79" t="n">
+        <v>77.45999999999999</v>
+      </c>
+      <c r="J79" t="n">
+        <v>9.960000000000001</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0</v>
+      </c>
+      <c r="C80" t="n">
+        <v>10.77</v>
+      </c>
+      <c r="D80" t="n">
+        <v>6.71</v>
+      </c>
+      <c r="E80" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="G80" t="n">
         <v>0.01</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="I80" t="n">
+        <v>13.7</v>
+      </c>
+      <c r="J80" t="n">
+        <v>6.32</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0</v>
+      </c>
+      <c r="C81" t="n">
+        <v>22.87</v>
+      </c>
+      <c r="D81" t="n">
+        <v>16.44</v>
+      </c>
+      <c r="E81" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="F81" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I81" t="n">
+        <v>55.55</v>
+      </c>
+      <c r="J81" t="n">
+        <v>7.45</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="n">
+        <v>1</v>
+      </c>
+      <c r="C82" t="n">
+        <v>78.31999999999999</v>
+      </c>
+      <c r="D82" t="n">
+        <v>22.26</v>
+      </c>
+      <c r="E82" t="n">
+        <v>6.54</v>
+      </c>
+      <c r="F82" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="I82" t="n">
+        <v>119.88</v>
+      </c>
+      <c r="J82" t="n">
+        <v>14.35</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0</v>
+      </c>
+      <c r="C83" t="n">
+        <v>19.02</v>
+      </c>
+      <c r="D83" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="E83" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="I83" t="n">
+        <v>32.25</v>
+      </c>
+      <c r="J83" t="n">
+        <v>7.41</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+      <c r="C84" t="n">
+        <v>8.140000000000001</v>
+      </c>
+      <c r="D84" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I84" t="n">
+        <v>10.47</v>
+      </c>
+      <c r="J84" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="n">
+        <v>1</v>
+      </c>
+      <c r="C85" t="n">
+        <v>43.52</v>
+      </c>
+      <c r="D85" t="n">
+        <v>18.49</v>
+      </c>
+      <c r="E85" t="n">
+        <v>6.38</v>
+      </c>
+      <c r="F85" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="I85" t="n">
+        <v>66.92</v>
+      </c>
+      <c r="J85" t="n">
+        <v>13.42</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>18.12</v>
+      </c>
+      <c r="D86" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="E86" t="n">
+        <v>2</v>
+      </c>
+      <c r="F86" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="G86" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I86" t="n">
+        <v>42.79</v>
+      </c>
+      <c r="J86" t="n">
+        <v>6.34</v>
+      </c>
+      <c r="K86" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0</v>
+      </c>
+      <c r="C87" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="D87" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="E87" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="F87" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="G87" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I87" t="n">
+        <v>47.54</v>
+      </c>
+      <c r="J87" t="n">
+        <v>6.58</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="n">
+        <v>1</v>
+      </c>
+      <c r="C88" t="n">
+        <v>52.89</v>
+      </c>
+      <c r="D88" t="n">
+        <v>27.84</v>
+      </c>
+      <c r="E88" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="F88" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I88" t="n">
+        <v>134.61</v>
+      </c>
+      <c r="J88" t="n">
+        <v>12.24</v>
+      </c>
+      <c r="K88" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0</v>
+      </c>
+      <c r="C89" t="n">
+        <v>9.01</v>
+      </c>
+      <c r="D89" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="E89" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I89" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="J89" t="n">
+        <v>5.41</v>
+      </c>
+      <c r="K89" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0</v>
+      </c>
+      <c r="C90" t="n">
+        <v>6.48</v>
+      </c>
+      <c r="D90" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="E90" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="G90" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I90" t="n">
+        <v>11</v>
+      </c>
+      <c r="J90" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="K90" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="n">
+        <v>1</v>
+      </c>
+      <c r="C91" t="n">
+        <v>46.68</v>
+      </c>
+      <c r="D91" t="n">
+        <v>15.31</v>
+      </c>
+      <c r="E91" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="F91" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="G91" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I91" t="n">
+        <v>85.94</v>
+      </c>
+      <c r="J91" t="n">
+        <v>9.93</v>
+      </c>
+      <c r="K91" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0</v>
+      </c>
+      <c r="C92" t="n">
+        <v>24.2</v>
+      </c>
+      <c r="D92" t="n">
+        <v>6.11</v>
+      </c>
+      <c r="E92" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="I92" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="J92" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="K92" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="n">
+        <v>1</v>
+      </c>
+      <c r="C93" t="n">
+        <v>72.84</v>
+      </c>
+      <c r="D93" t="n">
+        <v>36.33</v>
+      </c>
+      <c r="E93" t="n">
+        <v>9.869999999999999</v>
+      </c>
+      <c r="F93" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="G93" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="I93" t="n">
+        <v>200.66</v>
+      </c>
+      <c r="J93" t="n">
+        <v>20.86</v>
+      </c>
+      <c r="K93" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0</v>
+      </c>
+      <c r="C94" t="n">
+        <v>9.31</v>
+      </c>
+      <c r="D94" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E94" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I94" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="J94" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="K94" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0</v>
+      </c>
+      <c r="C95" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="D95" t="n">
+        <v>6.35</v>
+      </c>
+      <c r="E95" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="I95" t="n">
+        <v>26.16</v>
+      </c>
+      <c r="J95" t="n">
+        <v>5.94</v>
+      </c>
+      <c r="K95" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0</v>
+      </c>
+      <c r="C96" t="n">
+        <v>8.710000000000001</v>
+      </c>
+      <c r="D96" t="n">
+        <v>5.79</v>
+      </c>
+      <c r="E96" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="I96" t="n">
+        <v>14.43</v>
+      </c>
+      <c r="J96" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="K96" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0</v>
+      </c>
+      <c r="C97" t="n">
+        <v>7.31</v>
+      </c>
+      <c r="D97" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="E97" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="G97" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I97" t="n">
+        <v>9.94</v>
+      </c>
+      <c r="J97" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="K97" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="n">
+        <v>1</v>
+      </c>
+      <c r="C98" t="n">
+        <v>73.97</v>
+      </c>
+      <c r="D98" t="n">
+        <v>31.05</v>
+      </c>
+      <c r="E98" t="n">
+        <v>10.62</v>
+      </c>
+      <c r="F98" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="I98" t="n">
+        <v>136.74</v>
+      </c>
+      <c r="J98" t="n">
+        <v>21.91</v>
+      </c>
+      <c r="K98" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0</v>
+      </c>
+      <c r="C99" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="D99" t="n">
+        <v>7.23</v>
+      </c>
+      <c r="E99" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I99" t="n">
+        <v>18.32</v>
+      </c>
+      <c r="J99" t="n">
+        <v>6.26</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>